<commit_message>
Updated current status of UDQ screens
</commit_message>
<xml_diff>
--- a/OverallStatus.xlsx
+++ b/OverallStatus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="326" yWindow="27" windowWidth="23257" windowHeight="11425"/>
+    <workbookView xWindow="324" yWindow="24" windowWidth="23256" windowHeight="11424"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -699,10 +699,10 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -778,12 +778,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="192659456"/>
-        <c:axId val="162609344"/>
+        <c:axId val="183137792"/>
+        <c:axId val="175418176"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="192659456"/>
+        <c:axId val="183137792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,7 +792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162609344"/>
+        <c:crossAx val="175418176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -800,7 +800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162609344"/>
+        <c:axId val="175418176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="192659456"/>
+        <c:crossAx val="183137792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -935,10 +935,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1336,26 +1336,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.25" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.75" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="6" width="17.125" customWidth="1"/>
-    <col min="7" max="7" width="23.875" customWidth="1"/>
-    <col min="8" max="8" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
+    <col min="8" max="8" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>74</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1438,35 +1438,35 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>6</v>
+      <c r="D7" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="2">
         <f>COUNTIF(D5:D90,C2)</f>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J7" s="2">
         <f>COUNTIF(D5:D90,D2)</f>
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
@@ -1476,8 +1476,8 @@
       <c r="D8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>6</v>
+      <c r="E8" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>6</v>
@@ -1487,42 +1487,42 @@
       </c>
       <c r="I8" s="2">
         <f>COUNTIF(E5:E90,C2)</f>
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J8" s="2">
         <f>COUNTIF(E5:E90,D2)</f>
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>6</v>
+      <c r="D9" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="I9" s="2">
         <f>COUNTIF(F5:F90,C2)</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J9" s="2">
         <f>COUNTIF(F5:F90,D2)</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>19</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>23</v>
       </c>
@@ -1637,11 +1637,11 @@
       <c r="E16" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B20" s="23" t="s">
         <v>27</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>28</v>
       </c>
@@ -1722,11 +1722,11 @@
       <c r="E21" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
         <v>29</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
         <v>30</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>31</v>
       </c>
@@ -1777,24 +1777,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
         <v>33</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>34</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>35</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>36</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>37</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>38</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B32" s="24" t="s">
         <v>39</v>
       </c>
@@ -1913,92 +1913,92 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>6</v>
+      <c r="D33" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>6</v>
+      <c r="D34" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>6</v>
+      <c r="D35" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>6</v>
+      <c r="D36" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="F36" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>6</v>
+      <c r="D37" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B38" s="22" t="s">
         <v>45</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
         <v>75</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B40" s="21" t="s">
         <v>48</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="s">
         <v>49</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
         <v>45</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B43" s="9" t="s">
         <v>36</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
         <v>51</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" s="9" t="s">
         <v>13</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B46" s="9" t="s">
         <v>46</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
         <v>50</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B48" s="9" t="s">
         <v>52</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B49" s="9" t="s">
         <v>53</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="s">
         <v>54</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B51" s="9" t="s">
         <v>55</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B52" s="9" t="s">
         <v>56</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B53" s="9" t="s">
         <v>57</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
         <v>76</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B55" s="20" t="s">
         <v>5</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
         <v>59</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
         <v>60</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
         <v>61</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B59" s="10" t="s">
         <v>62</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
         <v>67</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="10" t="s">
         <v>63</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="10" t="s">
         <v>64</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B63" s="10" t="s">
         <v>65</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B64" s="10" t="s">
         <v>66</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="16" t="s">
         <v>77</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B66" s="11" t="s">
         <v>69</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B67" s="11" t="s">
         <v>70</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B68" s="11" t="s">
         <v>71</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B69" s="11" t="s">
         <v>72</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
         <v>78</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
         <v>79</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B72" s="5" t="s">
         <v>81</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
         <v>82</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B74" s="5" t="s">
         <v>83</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B75" s="5" t="s">
         <v>84</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B76" s="5" t="s">
         <v>85</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="29.25" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="16" t="s">
         <v>93</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B78" s="14" t="s">
         <v>87</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B79" s="14" t="s">
         <v>88</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B80" s="14" t="s">
         <v>89</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B81" s="14" t="s">
         <v>90</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B82" s="14" t="s">
         <v>91</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B83" s="14" t="s">
         <v>92</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="29.25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="16" t="s">
         <v>100</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B85" s="15" t="s">
         <v>95</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B86" s="15" t="s">
         <v>96</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B87" s="15" t="s">
         <v>97</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B88" s="15" t="s">
         <v>98</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B89" s="15" t="s">
         <v>99</v>
       </c>
@@ -2917,7 +2917,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2929,7 +2929,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated UDQ Companies status
</commit_message>
<xml_diff>
--- a/OverallStatus.xlsx
+++ b/OverallStatus.xlsx
@@ -699,10 +699,10 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -778,12 +778,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="183137792"/>
-        <c:axId val="175418176"/>
+        <c:axId val="184385024"/>
+        <c:axId val="174238528"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="183137792"/>
+        <c:axId val="184385024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,7 +792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175418176"/>
+        <c:crossAx val="174238528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -800,7 +800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175418176"/>
+        <c:axId val="174238528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183137792"/>
+        <c:crossAx val="184385024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1337,7 +1337,7 @@
   <dimension ref="A2:J89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,18 +1410,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>101</v>
+      <c r="D6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>7</v>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="I7" s="2">
         <f>COUNTIF(D5:D90,C2)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J7" s="2">
         <f>COUNTIF(D5:D90,D2)</f>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="I8" s="2">
         <f>COUNTIF(E5:E90,C2)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J8" s="2">
         <f>COUNTIF(E5:E90,D2)</f>

</xml_diff>

<commit_message>
Updated for Experience Rates Filter, Company code etc
</commit_message>
<xml_diff>
--- a/OverallStatus.xlsx
+++ b/OverallStatus.xlsx
@@ -699,10 +699,10 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -778,12 +778,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="184385024"/>
-        <c:axId val="174238528"/>
+        <c:axId val="187858432"/>
+        <c:axId val="177711936"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="184385024"/>
+        <c:axId val="187858432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,7 +792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174238528"/>
+        <c:crossAx val="177711936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -800,7 +800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174238528"/>
+        <c:axId val="177711936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184385024"/>
+        <c:crossAx val="187858432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1337,7 +1337,7 @@
   <dimension ref="A2:J89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="I7" s="2">
         <f>COUNTIF(D5:D90,C2)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J7" s="2">
         <f>COUNTIF(D5:D90,D2)</f>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="I8" s="2">
         <f>COUNTIF(E5:E90,C2)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J8" s="2">
         <f>COUNTIF(E5:E90,D2)</f>
@@ -1784,11 +1784,11 @@
       <c r="C25" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>101</v>
+      <c r="D25" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F25" s="18" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Updated Custom Overrides for Authority status
</commit_message>
<xml_diff>
--- a/OverallStatus.xlsx
+++ b/OverallStatus.xlsx
@@ -699,10 +699,10 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -778,12 +778,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="182812160"/>
-        <c:axId val="175090496"/>
+        <c:axId val="187465216"/>
+        <c:axId val="206834496"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="182812160"/>
+        <c:axId val="187465216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,7 +792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175090496"/>
+        <c:crossAx val="206834496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -800,7 +800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175090496"/>
+        <c:axId val="206834496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182812160"/>
+        <c:crossAx val="187465216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1336,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="I7" s="2">
         <f>COUNTIF(D5:D90,C2)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J7" s="2">
         <f>COUNTIF(D5:D90,D2)</f>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="I8" s="2">
         <f>COUNTIF(E5:E90,C2)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J8" s="2">
         <f>COUNTIF(E5:E90,D2)</f>
@@ -1971,11 +1971,11 @@
       <c r="C36" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>101</v>
+      <c r="D36" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F36" s="18" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Updated Ordered Percent Status
</commit_message>
<xml_diff>
--- a/OverallStatus.xlsx
+++ b/OverallStatus.xlsx
@@ -702,7 +702,7 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -778,12 +778,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="187465216"/>
-        <c:axId val="206834496"/>
+        <c:axId val="179731968"/>
+        <c:axId val="172010304"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="187465216"/>
+        <c:axId val="179731968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,7 +792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206834496"/>
+        <c:crossAx val="172010304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -800,7 +800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206834496"/>
+        <c:axId val="172010304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187465216"/>
+        <c:crossAx val="179731968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1336,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,8 +1476,8 @@
       <c r="D8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>101</v>
+      <c r="E8" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>6</v>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="I8" s="2">
         <f>COUNTIF(E5:E90,C2)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J8" s="2">
         <f>COUNTIF(E5:E90,D2)</f>

</xml_diff>

<commit_message>
updated overall sheet and added required error message to custom override for auth
</commit_message>
<xml_diff>
--- a/OverallStatus.xlsx
+++ b/OverallStatus.xlsx
@@ -1,27 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\git\tf-new-arch-artifacts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A91B26-C31F-42F1-8DFE-14BEE9CF22F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="324" yWindow="24" windowWidth="23256" windowHeight="11424"/>
+    <workbookView xWindow="9018" yWindow="858" windowWidth="15402" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Vinit Naik</author>
   </authors>
   <commentList>
-    <comment ref="B76" authorId="0">
+    <comment ref="B76" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -361,7 +377,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -609,12 +625,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -664,6 +683,13 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -671,6 +697,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -707,6 +738,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0070-4220-BA06-49DB25686467}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -724,6 +760,13 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -731,6 +774,11 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -767,6 +815,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0070-4220-BA06-49DB25686467}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -789,6 +842,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -818,7 +872,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -834,7 +887,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -848,7 +901,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -856,7 +908,6 @@
       <c:rotX val="30"/>
       <c:rotY val="0"/>
       <c:rAngAx val="0"/>
-      <c:perspective val="30"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -888,24 +939,41 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-FAEB-4BB5-8EDE-87C6C31F7080}"/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-FAEB-4BB5-8EDE-87C6C31F7080}"/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -913,6 +981,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -935,14 +1006,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FAEB-4BB5-8EDE-87C6C31F7080}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -957,7 +1033,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -999,7 +1074,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1029,7 +1110,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1090,7 +1177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1123,9 +1210,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1158,6 +1262,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1333,29 +1454,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.21875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" customWidth="1"/>
-    <col min="8" max="8" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.20703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1015625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.20703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7890625" customWidth="1"/>
+    <col min="5" max="5" width="17.68359375" customWidth="1"/>
+    <col min="6" max="6" width="17.1015625" customWidth="1"/>
+    <col min="7" max="7" width="23.89453125" customWidth="1"/>
+    <col min="8" max="8" width="24.20703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1015625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1366,7 +1485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="16" t="s">
         <v>74</v>
       </c>
@@ -1410,7 +1529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1438,7 +1557,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
@@ -1466,7 +1585,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
@@ -1494,7 +1613,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
@@ -1507,22 +1626,22 @@
       <c r="E9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>7</v>
+      <c r="F9" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="I9" s="2">
         <f>COUNTIF(F5:F90,C2)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J9" s="2">
         <f>COUNTIF(F5:F90,D2)</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
@@ -1539,7 +1658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
@@ -1556,7 +1675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="8" t="s">
         <v>19</v>
       </c>
@@ -1573,7 +1692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
@@ -1590,7 +1709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
@@ -1607,7 +1726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
@@ -1624,7 +1743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="8" t="s">
         <v>23</v>
       </c>
@@ -1637,11 +1756,11 @@
       <c r="E16" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="F16" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
@@ -1658,7 +1777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
@@ -1675,7 +1794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
@@ -1692,7 +1811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="23" t="s">
         <v>27</v>
       </c>
@@ -1709,7 +1828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="7" t="s">
         <v>28</v>
       </c>
@@ -1722,11 +1841,11 @@
       <c r="E21" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="F21" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="22" t="s">
         <v>29</v>
       </c>
@@ -1743,7 +1862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="27" t="s">
         <v>30</v>
       </c>
@@ -1760,7 +1879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="8" t="s">
         <v>31</v>
       </c>
@@ -1777,7 +1896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="7" t="s">
         <v>32</v>
       </c>
@@ -1794,7 +1913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="22" t="s">
         <v>33</v>
       </c>
@@ -1811,7 +1930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="7" t="s">
         <v>34</v>
       </c>
@@ -1828,7 +1947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="8" t="s">
         <v>35</v>
       </c>
@@ -1845,7 +1964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="7" t="s">
         <v>36</v>
       </c>
@@ -1862,7 +1981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="8" t="s">
         <v>37</v>
       </c>
@@ -1879,7 +1998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="8" t="s">
         <v>38</v>
       </c>
@@ -1896,7 +2015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="24" t="s">
         <v>39</v>
       </c>
@@ -1913,7 +2032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="7" t="s">
         <v>40</v>
       </c>
@@ -1930,7 +2049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="8" t="s">
         <v>41</v>
       </c>
@@ -1947,7 +2066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="7" t="s">
         <v>42</v>
       </c>
@@ -1964,7 +2083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="8" t="s">
         <v>43</v>
       </c>
@@ -1981,7 +2100,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="8" t="s">
         <v>44</v>
       </c>
@@ -1998,7 +2117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="22" t="s">
         <v>45</v>
       </c>
@@ -2015,7 +2134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="16" t="s">
         <v>75</v>
       </c>
@@ -2035,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="21" t="s">
         <v>48</v>
       </c>
@@ -2052,7 +2171,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="9" t="s">
         <v>49</v>
       </c>
@@ -2069,7 +2188,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="9" t="s">
         <v>45</v>
       </c>
@@ -2086,7 +2205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="9" t="s">
         <v>36</v>
       </c>
@@ -2103,7 +2222,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="9" t="s">
         <v>51</v>
       </c>
@@ -2120,7 +2239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="9" t="s">
         <v>13</v>
       </c>
@@ -2137,7 +2256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="9" t="s">
         <v>46</v>
       </c>
@@ -2154,7 +2273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="9" t="s">
         <v>50</v>
       </c>
@@ -2171,7 +2290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="9" t="s">
         <v>52</v>
       </c>
@@ -2188,7 +2307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="9" t="s">
         <v>53</v>
       </c>
@@ -2205,7 +2324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" s="9" t="s">
         <v>54</v>
       </c>
@@ -2222,7 +2341,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" s="9" t="s">
         <v>55</v>
       </c>
@@ -2239,7 +2358,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" s="9" t="s">
         <v>56</v>
       </c>
@@ -2256,7 +2375,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" s="9" t="s">
         <v>57</v>
       </c>
@@ -2273,7 +2392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="16" t="s">
         <v>76</v>
       </c>
@@ -2293,7 +2412,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" s="20" t="s">
         <v>5</v>
       </c>
@@ -2310,7 +2429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" s="10" t="s">
         <v>59</v>
       </c>
@@ -2327,7 +2446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="10" t="s">
         <v>60</v>
       </c>
@@ -2344,7 +2463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" s="10" t="s">
         <v>61</v>
       </c>
@@ -2361,7 +2480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" s="10" t="s">
         <v>62</v>
       </c>
@@ -2378,7 +2497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" s="10" t="s">
         <v>67</v>
       </c>
@@ -2395,7 +2514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" s="10" t="s">
         <v>63</v>
       </c>
@@ -2412,7 +2531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" s="10" t="s">
         <v>64</v>
       </c>
@@ -2429,7 +2548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" s="10" t="s">
         <v>65</v>
       </c>
@@ -2446,7 +2565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" s="10" t="s">
         <v>66</v>
       </c>
@@ -2463,7 +2582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="16" t="s">
         <v>77</v>
       </c>
@@ -2483,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" s="11" t="s">
         <v>69</v>
       </c>
@@ -2500,7 +2619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" s="11" t="s">
         <v>70</v>
       </c>
@@ -2517,7 +2636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" s="11" t="s">
         <v>71</v>
       </c>
@@ -2534,7 +2653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B69" s="11" t="s">
         <v>72</v>
       </c>
@@ -2551,7 +2670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="16" t="s">
         <v>78</v>
       </c>
@@ -2571,7 +2690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="16" t="s">
         <v>79</v>
       </c>
@@ -2591,7 +2710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B72" s="5" t="s">
         <v>81</v>
       </c>
@@ -2608,7 +2727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B73" s="5" t="s">
         <v>82</v>
       </c>
@@ -2625,7 +2744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" s="5" t="s">
         <v>83</v>
       </c>
@@ -2642,7 +2761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" s="5" t="s">
         <v>84</v>
       </c>
@@ -2659,7 +2778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B76" s="5" t="s">
         <v>85</v>
       </c>
@@ -2676,7 +2795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A77" s="16" t="s">
         <v>93</v>
       </c>
@@ -2696,7 +2815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B78" s="14" t="s">
         <v>87</v>
       </c>
@@ -2713,7 +2832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B79" s="14" t="s">
         <v>88</v>
       </c>
@@ -2730,7 +2849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B80" s="14" t="s">
         <v>89</v>
       </c>
@@ -2747,7 +2866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B81" s="14" t="s">
         <v>90</v>
       </c>
@@ -2764,7 +2883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B82" s="14" t="s">
         <v>91</v>
       </c>
@@ -2781,7 +2900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B83" s="14" t="s">
         <v>92</v>
       </c>
@@ -2798,7 +2917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="29.1" x14ac:dyDescent="0.6">
       <c r="A84" s="16" t="s">
         <v>100</v>
       </c>
@@ -2818,7 +2937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B85" s="15" t="s">
         <v>95</v>
       </c>
@@ -2835,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B86" s="15" t="s">
         <v>96</v>
       </c>
@@ -2852,7 +2971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B87" s="15" t="s">
         <v>97</v>
       </c>
@@ -2869,7 +2988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B88" s="15" t="s">
         <v>98</v>
       </c>
@@ -2886,7 +3005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B89" s="15" t="s">
         <v>99</v>
       </c>
@@ -2912,24 +3031,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated status for UDQ pages
</commit_message>
<xml_diff>
--- a/OverallStatus.xlsx
+++ b/OverallStatus.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\git\tf-new-arch-artifacts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A91B26-C31F-42F1-8DFE-14BEE9CF22F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9018" yWindow="858" windowWidth="15402" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9024" yWindow="864" windowWidth="15408" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Vinit Naik</author>
   </authors>
   <commentList>
-    <comment ref="B76" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="101">
   <si>
     <t>UI/Screen</t>
   </si>
@@ -369,15 +363,12 @@
   </si>
   <si>
     <t>External Link Areas</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -554,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -594,17 +585,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -612,9 +596,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +614,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -697,7 +678,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -727,18 +708,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>54</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0070-4220-BA06-49DB25686467}"/>
             </c:ext>
@@ -774,7 +755,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -807,15 +788,15 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0070-4220-BA06-49DB25686467}"/>
             </c:ext>
@@ -831,12 +812,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="179731968"/>
-        <c:axId val="172010304"/>
+        <c:axId val="175160320"/>
+        <c:axId val="194513152"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="179731968"/>
+        <c:axId val="175160320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +827,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172010304"/>
+        <c:crossAx val="194513152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -854,7 +835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172010304"/>
+        <c:axId val="194513152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -865,13 +846,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179731968"/>
+        <c:crossAx val="175160320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -887,7 +869,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -901,6 +883,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -908,6 +891,7 @@
       <c:rotX val="30"/>
       <c:rotY val="0"/>
       <c:rAngAx val="0"/>
+      <c:perspective val="30"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -939,13 +923,14 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-FAEB-4BB5-8EDE-87C6C31F7080}"/>
@@ -954,13 +939,14 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-FAEB-4BB5-8EDE-87C6C31F7080}"/>
@@ -981,7 +967,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -1014,7 +1000,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-FAEB-4BB5-8EDE-87C6C31F7080}"/>
             </c:ext>
@@ -1033,6 +1019,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1077,7 +1064,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1113,7 +1100,7 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1177,7 +1164,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1210,26 +1197,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1262,23 +1232,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1454,38 +1407,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.20703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.1015625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.20703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7890625" customWidth="1"/>
-    <col min="5" max="5" width="17.68359375" customWidth="1"/>
-    <col min="6" max="6" width="17.1015625" customWidth="1"/>
-    <col min="7" max="7" width="23.89453125" customWidth="1"/>
-    <col min="8" max="8" width="24.20703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" customWidth="1"/>
+    <col min="8" max="8" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.89453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>74</v>
       </c>
@@ -1529,7 +1484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1550,25 +1505,25 @@
       </c>
       <c r="I6" s="2">
         <f>COUNTIF(C5:C90,C2)</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J6" s="2">
         <f>COUNTIF(C5:C90,D2)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>101</v>
+      <c r="D7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>7</v>
@@ -1578,14 +1533,14 @@
       </c>
       <c r="I7" s="2">
         <f>COUNTIF(D5:D90,C2)</f>
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="J7" s="2">
         <f>COUNTIF(D5:D90,D2)</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
@@ -1606,14 +1561,14 @@
       </c>
       <c r="I8" s="2">
         <f>COUNTIF(E5:E90,C2)</f>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J8" s="2">
         <f>COUNTIF(E5:E90,D2)</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
@@ -1641,7 +1596,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
@@ -1658,7 +1613,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
@@ -1675,7 +1630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>19</v>
       </c>
@@ -1692,7 +1647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
@@ -1709,7 +1664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
@@ -1726,7 +1681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
@@ -1743,7 +1698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>23</v>
       </c>
@@ -1760,7 +1715,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
@@ -1777,8 +1732,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="8" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="17" t="s">
@@ -1794,7 +1749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
@@ -1811,8 +1766,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="23" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="17" t="s">
@@ -1828,7 +1783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>28</v>
       </c>
@@ -1845,8 +1800,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="22" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="17" t="s">
@@ -1862,8 +1817,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="27" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="17" t="s">
@@ -1879,8 +1834,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" s="8" t="s">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="17" t="s">
@@ -1896,7 +1851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>32</v>
       </c>
@@ -1913,8 +1868,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="22" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="17" t="s">
@@ -1930,7 +1885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>34</v>
       </c>
@@ -1947,8 +1902,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" s="8" t="s">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="17" t="s">
@@ -1964,7 +1919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
         <v>36</v>
       </c>
@@ -1981,8 +1936,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="8" t="s">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="17" t="s">
@@ -1998,25 +1953,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>7</v>
+      <c r="C31" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="24" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="21" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="17" t="s">
@@ -2032,58 +1987,58 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>101</v>
+      <c r="D33" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>101</v>
+      <c r="D34" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>101</v>
+      <c r="D35" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
         <v>43</v>
       </c>
@@ -2100,25 +2055,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>101</v>
+      <c r="D37" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38" s="22" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="17" t="s">
@@ -2134,11 +2089,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="20" t="s">
         <v>47</v>
       </c>
       <c r="C39" s="17" t="s">
@@ -2154,8 +2109,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40" s="21" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="20" t="s">
         <v>48</v>
       </c>
       <c r="C40" s="17" t="s">
@@ -2171,7 +2126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="s">
         <v>49</v>
       </c>
@@ -2188,7 +2143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
         <v>45</v>
       </c>
@@ -2205,7 +2160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B43" s="9" t="s">
         <v>36</v>
       </c>
@@ -2222,7 +2177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
         <v>51</v>
       </c>
@@ -2239,7 +2194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" s="9" t="s">
         <v>13</v>
       </c>
@@ -2256,7 +2211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B46" s="9" t="s">
         <v>46</v>
       </c>
@@ -2273,7 +2228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
         <v>50</v>
       </c>
@@ -2290,7 +2245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B48" s="9" t="s">
         <v>52</v>
       </c>
@@ -2307,7 +2262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B49" s="9" t="s">
         <v>53</v>
       </c>
@@ -2324,7 +2279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="s">
         <v>54</v>
       </c>
@@ -2341,7 +2296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B51" s="9" t="s">
         <v>55</v>
       </c>
@@ -2358,7 +2313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B52" s="9" t="s">
         <v>56</v>
       </c>
@@ -2375,7 +2330,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B53" s="9" t="s">
         <v>57</v>
       </c>
@@ -2392,11 +2347,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="19" t="s">
         <v>58</v>
       </c>
       <c r="C54" s="17" t="s">
@@ -2412,8 +2367,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B55" s="20" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="17" t="s">
@@ -2429,7 +2384,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
         <v>59</v>
       </c>
@@ -2446,7 +2401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
         <v>60</v>
       </c>
@@ -2463,7 +2418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
         <v>61</v>
       </c>
@@ -2480,7 +2435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B59" s="10" t="s">
         <v>62</v>
       </c>
@@ -2497,7 +2452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
         <v>67</v>
       </c>
@@ -2514,7 +2469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="10" t="s">
         <v>63</v>
       </c>
@@ -2531,7 +2486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="10" t="s">
         <v>64</v>
       </c>
@@ -2548,7 +2503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B63" s="10" t="s">
         <v>65</v>
       </c>
@@ -2565,7 +2520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B64" s="10" t="s">
         <v>66</v>
       </c>
@@ -2582,7 +2537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="16" t="s">
         <v>77</v>
       </c>
@@ -2602,7 +2557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B66" s="11" t="s">
         <v>69</v>
       </c>
@@ -2619,7 +2574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B67" s="11" t="s">
         <v>70</v>
       </c>
@@ -2636,7 +2591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B68" s="11" t="s">
         <v>71</v>
       </c>
@@ -2653,7 +2608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B69" s="11" t="s">
         <v>72</v>
       </c>
@@ -2670,7 +2625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
         <v>78</v>
       </c>
@@ -2690,7 +2645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
         <v>79</v>
       </c>
@@ -2710,7 +2665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B72" s="5" t="s">
         <v>81</v>
       </c>
@@ -2727,7 +2682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
         <v>82</v>
       </c>
@@ -2744,7 +2699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B74" s="5" t="s">
         <v>83</v>
       </c>
@@ -2761,7 +2716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B75" s="5" t="s">
         <v>84</v>
       </c>
@@ -2778,7 +2733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B76" s="5" t="s">
         <v>85</v>
       </c>
@@ -2795,7 +2750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="16" t="s">
         <v>93</v>
       </c>
@@ -2815,7 +2770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B78" s="14" t="s">
         <v>87</v>
       </c>
@@ -2832,7 +2787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="79" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B79" s="14" t="s">
         <v>88</v>
       </c>
@@ -2849,7 +2804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B80" s="14" t="s">
         <v>89</v>
       </c>
@@ -2866,7 +2821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="81" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B81" s="14" t="s">
         <v>90</v>
       </c>
@@ -2883,7 +2838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="82" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B82" s="14" t="s">
         <v>91</v>
       </c>
@@ -2900,7 +2855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="83" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B83" s="14" t="s">
         <v>92</v>
       </c>
@@ -2917,7 +2872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="29.1" x14ac:dyDescent="0.6">
+    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="16" t="s">
         <v>100</v>
       </c>
@@ -2937,7 +2892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="85" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B85" s="15" t="s">
         <v>95</v>
       </c>
@@ -2954,7 +2909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="86" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B86" s="15" t="s">
         <v>96</v>
       </c>
@@ -2971,7 +2926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="87" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B87" s="15" t="s">
         <v>97</v>
       </c>
@@ -2988,7 +2943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="88" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B88" s="15" t="s">
         <v>98</v>
       </c>
@@ -3005,7 +2960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="89" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B89" s="15" t="s">
         <v>99</v>
       </c>
@@ -3031,24 +2986,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated overall status excel sheet
</commit_message>
<xml_diff>
--- a/OverallStatus.xlsx
+++ b/OverallStatus.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\git\tf-new-arch-artifacts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62AA126-CB82-4596-A173-6AAE80C42BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9024" yWindow="864" windowWidth="15408" windowHeight="9000"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Vinit Naik</author>
   </authors>
   <commentList>
-    <comment ref="B76" authorId="0">
+    <comment ref="B76" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -368,7 +374,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -614,7 +620,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -678,7 +684,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -719,7 +725,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0070-4220-BA06-49DB25686467}"/>
             </c:ext>
@@ -755,7 +761,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -796,7 +802,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0070-4220-BA06-49DB25686467}"/>
             </c:ext>
@@ -853,7 +859,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -869,7 +874,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -883,7 +888,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -891,7 +895,6 @@
       <c:rotX val="30"/>
       <c:rotY val="0"/>
       <c:rAngAx val="0"/>
-      <c:perspective val="30"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -923,14 +926,13 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-FAEB-4BB5-8EDE-87C6C31F7080}"/>
@@ -939,14 +941,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-FAEB-4BB5-8EDE-87C6C31F7080}"/>
@@ -967,7 +968,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -992,15 +993,15 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-FAEB-4BB5-8EDE-87C6C31F7080}"/>
             </c:ext>
@@ -1019,7 +1020,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1064,7 +1064,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1100,7 +1100,7 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1164,7 +1164,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1197,9 +1197,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1232,6 +1249,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1407,29 +1441,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.21875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" customWidth="1"/>
-    <col min="8" max="8" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.20703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1015625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.20703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7890625" customWidth="1"/>
+    <col min="5" max="5" width="17.68359375" customWidth="1"/>
+    <col min="6" max="6" width="17.1015625" customWidth="1"/>
+    <col min="7" max="7" width="23.89453125" customWidth="1"/>
+    <col min="8" max="8" width="24.20703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1015625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1440,7 +1474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1457,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="16" t="s">
         <v>74</v>
       </c>
@@ -1484,7 +1518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1512,7 +1546,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
@@ -1540,7 +1574,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
@@ -1568,7 +1602,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
@@ -1589,14 +1623,14 @@
       </c>
       <c r="I9" s="2">
         <f>COUNTIF(F5:F90,C2)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J9" s="2">
         <f>COUNTIF(F5:F90,D2)</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
@@ -1613,7 +1647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
@@ -1630,7 +1664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="8" t="s">
         <v>19</v>
       </c>
@@ -1647,7 +1681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="7" t="s">
         <v>20</v>
       </c>
@@ -1664,7 +1698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
@@ -1681,7 +1715,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
@@ -1698,7 +1732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="8" t="s">
         <v>23</v>
       </c>
@@ -1715,7 +1749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
@@ -1732,7 +1766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
@@ -1749,7 +1783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
@@ -1766,7 +1800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="7" t="s">
         <v>27</v>
       </c>
@@ -1783,7 +1817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="7" t="s">
         <v>28</v>
       </c>
@@ -1800,7 +1834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
@@ -1817,7 +1851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="7" t="s">
         <v>30</v>
       </c>
@@ -1834,7 +1868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="7" t="s">
         <v>31</v>
       </c>
@@ -1851,7 +1885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="7" t="s">
         <v>32</v>
       </c>
@@ -1868,7 +1902,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="7" t="s">
         <v>33</v>
       </c>
@@ -1885,7 +1919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="7" t="s">
         <v>34</v>
       </c>
@@ -1902,7 +1936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="7" t="s">
         <v>35</v>
       </c>
@@ -1919,7 +1953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="7" t="s">
         <v>36</v>
       </c>
@@ -1936,7 +1970,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="7" t="s">
         <v>37</v>
       </c>
@@ -1953,7 +1987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="8" t="s">
         <v>38</v>
       </c>
@@ -1970,7 +2004,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="21" t="s">
         <v>39</v>
       </c>
@@ -1983,11 +2017,11 @@
       <c r="E32" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F32" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="7" t="s">
         <v>40</v>
       </c>
@@ -2004,7 +2038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="8" t="s">
         <v>41</v>
       </c>
@@ -2021,7 +2055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="7" t="s">
         <v>42</v>
       </c>
@@ -2034,11 +2068,11 @@
       <c r="E35" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F35" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="8" t="s">
         <v>43</v>
       </c>
@@ -2055,7 +2089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="8" t="s">
         <v>44</v>
       </c>
@@ -2072,7 +2106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="8" t="s">
         <v>45</v>
       </c>
@@ -2089,7 +2123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="16" t="s">
         <v>75</v>
       </c>
@@ -2109,7 +2143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="20" t="s">
         <v>48</v>
       </c>
@@ -2126,7 +2160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="9" t="s">
         <v>49</v>
       </c>
@@ -2143,7 +2177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="9" t="s">
         <v>45</v>
       </c>
@@ -2160,7 +2194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="9" t="s">
         <v>36</v>
       </c>
@@ -2177,7 +2211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="9" t="s">
         <v>51</v>
       </c>
@@ -2194,7 +2228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="9" t="s">
         <v>13</v>
       </c>
@@ -2211,7 +2245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="9" t="s">
         <v>46</v>
       </c>
@@ -2228,7 +2262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="9" t="s">
         <v>50</v>
       </c>
@@ -2245,7 +2279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="9" t="s">
         <v>52</v>
       </c>
@@ -2262,7 +2296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="9" t="s">
         <v>53</v>
       </c>
@@ -2279,7 +2313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" s="9" t="s">
         <v>54</v>
       </c>
@@ -2296,7 +2330,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" s="9" t="s">
         <v>55</v>
       </c>
@@ -2313,7 +2347,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" s="9" t="s">
         <v>56</v>
       </c>
@@ -2330,7 +2364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" s="9" t="s">
         <v>57</v>
       </c>
@@ -2347,7 +2381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="16" t="s">
         <v>76</v>
       </c>
@@ -2367,7 +2401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" s="19" t="s">
         <v>5</v>
       </c>
@@ -2384,7 +2418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" s="10" t="s">
         <v>59</v>
       </c>
@@ -2401,7 +2435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="10" t="s">
         <v>60</v>
       </c>
@@ -2418,7 +2452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" s="10" t="s">
         <v>61</v>
       </c>
@@ -2435,7 +2469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" s="10" t="s">
         <v>62</v>
       </c>
@@ -2452,7 +2486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" s="10" t="s">
         <v>67</v>
       </c>
@@ -2469,7 +2503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" s="10" t="s">
         <v>63</v>
       </c>
@@ -2486,7 +2520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" s="10" t="s">
         <v>64</v>
       </c>
@@ -2503,7 +2537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" s="10" t="s">
         <v>65</v>
       </c>
@@ -2520,7 +2554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" s="10" t="s">
         <v>66</v>
       </c>
@@ -2537,7 +2571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="16" t="s">
         <v>77</v>
       </c>
@@ -2557,7 +2591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" s="11" t="s">
         <v>69</v>
       </c>
@@ -2574,7 +2608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" s="11" t="s">
         <v>70</v>
       </c>
@@ -2591,7 +2625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" s="11" t="s">
         <v>71</v>
       </c>
@@ -2608,7 +2642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B69" s="11" t="s">
         <v>72</v>
       </c>
@@ -2625,7 +2659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="16" t="s">
         <v>78</v>
       </c>
@@ -2645,7 +2679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="16" t="s">
         <v>79</v>
       </c>
@@ -2665,7 +2699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B72" s="5" t="s">
         <v>81</v>
       </c>
@@ -2682,7 +2716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B73" s="5" t="s">
         <v>82</v>
       </c>
@@ -2699,7 +2733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" s="5" t="s">
         <v>83</v>
       </c>
@@ -2716,7 +2750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" s="5" t="s">
         <v>84</v>
       </c>
@@ -2733,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B76" s="5" t="s">
         <v>85</v>
       </c>
@@ -2750,7 +2784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A77" s="16" t="s">
         <v>93</v>
       </c>
@@ -2770,7 +2804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B78" s="14" t="s">
         <v>87</v>
       </c>
@@ -2787,7 +2821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B79" s="14" t="s">
         <v>88</v>
       </c>
@@ -2804,7 +2838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B80" s="14" t="s">
         <v>89</v>
       </c>
@@ -2821,7 +2855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B81" s="14" t="s">
         <v>90</v>
       </c>
@@ -2838,7 +2872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B82" s="14" t="s">
         <v>91</v>
       </c>
@@ -2855,7 +2889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B83" s="14" t="s">
         <v>92</v>
       </c>
@@ -2872,7 +2906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="29.1" x14ac:dyDescent="0.6">
       <c r="A84" s="16" t="s">
         <v>100</v>
       </c>
@@ -2892,7 +2926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B85" s="15" t="s">
         <v>95</v>
       </c>
@@ -2909,7 +2943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B86" s="15" t="s">
         <v>96</v>
       </c>
@@ -2926,7 +2960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B87" s="15" t="s">
         <v>97</v>
       </c>
@@ -2943,7 +2977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B88" s="15" t="s">
         <v>98</v>
       </c>
@@ -2960,7 +2994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="15.6" x14ac:dyDescent="0.6">
       <c r="B89" s="15" t="s">
         <v>99</v>
       </c>
@@ -2986,24 +3020,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>